<commit_message>
Added ooxml jar to pom
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinay/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinay/IdeaProjects/CucumberProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DBADAD1-0238-5F4C-8D53-35A9D703C7F9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CD5D95F-05E7-4947-8306-B05B2545D80A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16380" xr2:uid="{92C796A7-57AD-8748-941B-403BFDC8F118}"/>
   </bookViews>

</xml_diff>

<commit_message>
Added new jdbc jar
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vinay Gopinath\git\CucumberMaven\"/>
     </mc:Choice>
@@ -16,7 +16,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="2">
   <si>
     <t>Selenium Core</t>
   </si>
@@ -36,6 +36,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -381,13 +382,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.0" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -398,6 +399,11 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2">
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>